<commit_message>
joins created lookup table, cleans up inconsistent names
</commit_message>
<xml_diff>
--- a/data-raw/snorkel_built_lookup_table.xlsx
+++ b/data-raw/snorkel_built_lookup_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD27128A-7895-49E1-9AE6-71D387AD700C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F01990A-4FD0-47A1-A7BD-2C9A9AF25E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9470" yWindow="670" windowWidth="14860" windowHeight="14340" xr2:uid="{587829D2-FD03-4E25-88F1-9BE0668E98CA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="29">
   <si>
     <t>unit</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>McFarland</t>
+  </si>
+  <si>
+    <t>sample_type</t>
+  </si>
+  <si>
+    <t>permanent</t>
   </si>
 </sst>
 </file>
@@ -494,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24ADAE37-2B29-4182-897B-2B0088CFE770}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -505,7 +511,7 @@
     <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,8 +521,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>23</v>
       </c>
@@ -526,8 +535,11 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>24</v>
       </c>
@@ -537,8 +549,11 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>25</v>
       </c>
@@ -548,8 +563,11 @@
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>19</v>
       </c>
@@ -559,8 +577,11 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>26</v>
       </c>
@@ -570,8 +591,11 @@
       <c r="C6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>28</v>
       </c>
@@ -581,8 +605,11 @@
       <c r="C7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>33</v>
       </c>
@@ -592,8 +619,11 @@
       <c r="C8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>29</v>
       </c>
@@ -603,8 +633,11 @@
       <c r="C9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>30</v>
       </c>
@@ -614,8 +647,11 @@
       <c r="C10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>31</v>
       </c>
@@ -625,8 +661,11 @@
       <c r="C11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>32</v>
       </c>
@@ -636,8 +675,11 @@
       <c r="C12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>55</v>
       </c>
@@ -647,8 +689,11 @@
       <c r="C13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>56</v>
       </c>
@@ -658,8 +703,11 @@
       <c r="C14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>96</v>
       </c>
@@ -669,8 +717,11 @@
       <c r="C15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>97</v>
       </c>
@@ -680,8 +731,11 @@
       <c r="C16">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>98</v>
       </c>
@@ -691,8 +745,11 @@
       <c r="C17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>103</v>
       </c>
@@ -702,8 +759,11 @@
       <c r="C18">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>104</v>
       </c>
@@ -713,8 +773,11 @@
       <c r="C19">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>105</v>
       </c>
@@ -724,8 +787,11 @@
       <c r="C20">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>119</v>
       </c>
@@ -735,8 +801,11 @@
       <c r="C21">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>120</v>
       </c>
@@ -746,8 +815,11 @@
       <c r="C22">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>169</v>
       </c>
@@ -757,8 +829,11 @@
       <c r="C23">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>170</v>
       </c>
@@ -768,8 +843,11 @@
       <c r="C24">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>171</v>
       </c>
@@ -779,8 +857,11 @@
       <c r="C25">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>173</v>
       </c>
@@ -790,8 +871,11 @@
       <c r="C26">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>174</v>
       </c>
@@ -801,8 +885,11 @@
       <c r="C27">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>175</v>
       </c>
@@ -812,8 +899,11 @@
       <c r="C28">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>185</v>
       </c>
@@ -823,8 +913,11 @@
       <c r="C29">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>189</v>
       </c>
@@ -834,8 +927,11 @@
       <c r="C30">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -845,8 +941,11 @@
       <c r="C31">
         <v>11</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>216</v>
       </c>
@@ -856,8 +955,11 @@
       <c r="C32">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -867,8 +969,11 @@
       <c r="C33">
         <v>11</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>217</v>
       </c>
@@ -878,8 +983,11 @@
       <c r="C34">
         <v>11</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>210</v>
       </c>
@@ -889,8 +997,11 @@
       <c r="C35">
         <v>11</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>221</v>
       </c>
@@ -900,8 +1011,11 @@
       <c r="C36">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>225</v>
       </c>
@@ -911,8 +1025,11 @@
       <c r="C37">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>226</v>
       </c>
@@ -922,8 +1039,11 @@
       <c r="C38">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>229</v>
       </c>
@@ -933,8 +1053,11 @@
       <c r="C39">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>228</v>
       </c>
@@ -944,8 +1067,11 @@
       <c r="C40">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>268</v>
       </c>
@@ -955,8 +1081,11 @@
       <c r="C41">
         <v>13</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>266</v>
       </c>
@@ -966,8 +1095,11 @@
       <c r="C42">
         <v>13</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -977,8 +1109,11 @@
       <c r="C43">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>25</v>
       </c>
@@ -988,8 +1123,11 @@
       <c r="C44">
         <v>14</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>402</v>
       </c>
@@ -999,8 +1137,11 @@
       <c r="C45">
         <v>15</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>403</v>
       </c>
@@ -1010,8 +1151,11 @@
       <c r="C46">
         <v>15</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>397</v>
       </c>
@@ -1021,8 +1165,11 @@
       <c r="C47">
         <v>15</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>408</v>
       </c>
@@ -1032,8 +1179,11 @@
       <c r="C48">
         <v>16</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>424</v>
       </c>
@@ -1043,8 +1193,11 @@
       <c r="C49">
         <v>17</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>426</v>
       </c>
@@ -1054,8 +1207,11 @@
       <c r="C50">
         <v>17</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>441</v>
       </c>
@@ -1065,8 +1221,11 @@
       <c r="C51">
         <v>18</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D51" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>445</v>
       </c>
@@ -1076,8 +1235,11 @@
       <c r="C52">
         <v>18</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>450</v>
       </c>
@@ -1087,8 +1249,11 @@
       <c r="C53">
         <v>18</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D53" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>486</v>
       </c>
@@ -1098,8 +1263,11 @@
       <c r="C54">
         <v>19</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D54" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>487</v>
       </c>
@@ -1109,8 +1277,11 @@
       <c r="C55">
         <v>19</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D55" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>499</v>
       </c>
@@ -1120,8 +1291,11 @@
       <c r="C56">
         <v>20</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D56" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>502</v>
       </c>
@@ -1130,6 +1304,9 @@
       </c>
       <c r="C57">
         <v>20</v>
+      </c>
+      <c r="D57" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>